<commit_message>
USA_main to loop; switch function for yield filter assembly to sector IDs; correct filter spelling mistake
switch function for yield filter assembly to sector ID: function was using sector labels before, which led to errors as some sector labels were the same despite having different IDs (=being different sectors)
</commit_message>
<xml_diff>
--- a/input_data/USA/Filter_2002_Base.xlsx
+++ b/input_data/USA/Filter_2002_Base.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE69C269-F9A6-4D27-88AB-F569A1272ACE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B598F9C-7C17-4FFB-BD6B-3CD76B6BE247}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12228" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -547,7 +547,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="963">
   <si>
     <t>Oilseed farming</t>
   </si>
@@ -3424,9 +3424,6 @@
   </si>
   <si>
     <t>USA</t>
-  </si>
-  <si>
-    <t>Other buildungs</t>
   </si>
   <si>
     <t>Wood</t>
@@ -4219,34 +4216,34 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>888</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>889</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>882</v>
       </c>
@@ -4254,7 +4251,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>283</v>
       </c>
@@ -4262,7 +4259,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>296</v>
       </c>
@@ -4270,7 +4267,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>295</v>
       </c>
@@ -4278,7 +4275,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>294</v>
       </c>
@@ -4286,7 +4283,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="15" spans="2:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
@@ -4294,10 +4291,10 @@
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="13"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>902</v>
       </c>
@@ -4311,20 +4308,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB432"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C320" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A181" sqref="A181:B185"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="52.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="52.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>287</v>
       </c>
@@ -4352,7 +4349,7 @@
       <c r="Y1" s="76"/>
       <c r="Z1" s="76"/>
     </row>
-    <row r="2" spans="1:28" ht="133.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="128.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
         <v>896</v>
       </c>
@@ -4438,7 +4435,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>452</v>
       </c>
@@ -4526,7 +4523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>453</v>
       </c>
@@ -4614,7 +4611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>454</v>
       </c>
@@ -4702,7 +4699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>455</v>
       </c>
@@ -4790,7 +4787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>456</v>
       </c>
@@ -4878,7 +4875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>457</v>
       </c>
@@ -4966,7 +4963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>458</v>
       </c>
@@ -5054,7 +5051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>459</v>
       </c>
@@ -5142,7 +5139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>460</v>
       </c>
@@ -5230,7 +5227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>461</v>
       </c>
@@ -5318,7 +5315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>462</v>
       </c>
@@ -5406,7 +5403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>463</v>
       </c>
@@ -5494,7 +5491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>464</v>
       </c>
@@ -5582,7 +5579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>465</v>
       </c>
@@ -5670,7 +5667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>466</v>
       </c>
@@ -5758,7 +5755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>467</v>
       </c>
@@ -5846,7 +5843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>468</v>
       </c>
@@ -5934,7 +5931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>469</v>
       </c>
@@ -6022,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>470</v>
       </c>
@@ -6110,7 +6107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>471</v>
       </c>
@@ -6198,7 +6195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>472</v>
       </c>
@@ -6286,7 +6283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>473</v>
       </c>
@@ -6374,7 +6371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>474</v>
       </c>
@@ -6462,7 +6459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>475</v>
       </c>
@@ -6550,7 +6547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>476</v>
       </c>
@@ -6638,7 +6635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>477</v>
       </c>
@@ -6726,7 +6723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>478</v>
       </c>
@@ -6814,7 +6811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>479</v>
       </c>
@@ -6902,7 +6899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>480</v>
       </c>
@@ -6990,7 +6987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>481</v>
       </c>
@@ -7078,7 +7075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>482</v>
       </c>
@@ -7166,7 +7163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>483</v>
       </c>
@@ -7254,7 +7251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>484</v>
       </c>
@@ -7342,7 +7339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
         <v>485</v>
       </c>
@@ -7430,7 +7427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>486</v>
       </c>
@@ -7518,7 +7515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>487</v>
       </c>
@@ -7606,7 +7603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" s="21" t="s">
         <v>488</v>
       </c>
@@ -7694,7 +7691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>489</v>
       </c>
@@ -7782,7 +7779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>490</v>
       </c>
@@ -7870,7 +7867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="21" t="s">
         <v>491</v>
       </c>
@@ -7958,7 +7955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>492</v>
       </c>
@@ -8046,7 +8043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>493</v>
       </c>
@@ -8134,7 +8131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>494</v>
       </c>
@@ -8222,7 +8219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>495</v>
       </c>
@@ -8310,7 +8307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>496</v>
       </c>
@@ -8398,7 +8395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>497</v>
       </c>
@@ -8486,7 +8483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>498</v>
       </c>
@@ -8574,7 +8571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>499</v>
       </c>
@@ -8662,7 +8659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>500</v>
       </c>
@@ -8750,7 +8747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>501</v>
       </c>
@@ -8838,7 +8835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>502</v>
       </c>
@@ -8926,7 +8923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>503</v>
       </c>
@@ -9014,7 +9011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>504</v>
       </c>
@@ -9102,7 +9099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>505</v>
       </c>
@@ -9190,7 +9187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>506</v>
       </c>
@@ -9278,7 +9275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>507</v>
       </c>
@@ -9366,7 +9363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>508</v>
       </c>
@@ -9454,7 +9451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>509</v>
       </c>
@@ -9542,7 +9539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>510</v>
       </c>
@@ -9630,7 +9627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>511</v>
       </c>
@@ -9718,7 +9715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>512</v>
       </c>
@@ -9806,7 +9803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>513</v>
       </c>
@@ -9894,7 +9891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>514</v>
       </c>
@@ -9982,7 +9979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>515</v>
       </c>
@@ -10070,7 +10067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>516</v>
       </c>
@@ -10158,7 +10155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>517</v>
       </c>
@@ -10246,7 +10243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>518</v>
       </c>
@@ -10334,7 +10331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>519</v>
       </c>
@@ -10422,7 +10419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>520</v>
       </c>
@@ -10510,7 +10507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>521</v>
       </c>
@@ -10598,7 +10595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>522</v>
       </c>
@@ -10686,7 +10683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>523</v>
       </c>
@@ -10774,7 +10771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>524</v>
       </c>
@@ -10862,7 +10859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>525</v>
       </c>
@@ -10950,7 +10947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>526</v>
       </c>
@@ -11038,7 +11035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>527</v>
       </c>
@@ -11126,7 +11123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>528</v>
       </c>
@@ -11214,7 +11211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>529</v>
       </c>
@@ -11302,7 +11299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>530</v>
       </c>
@@ -11390,7 +11387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>531</v>
       </c>
@@ -11478,7 +11475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>532</v>
       </c>
@@ -11566,7 +11563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>533</v>
       </c>
@@ -11654,7 +11651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>534</v>
       </c>
@@ -11742,7 +11739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>535</v>
       </c>
@@ -11830,7 +11827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>536</v>
       </c>
@@ -11918,7 +11915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>537</v>
       </c>
@@ -12006,7 +12003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>538</v>
       </c>
@@ -12094,7 +12091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>539</v>
       </c>
@@ -12182,7 +12179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>540</v>
       </c>
@@ -12270,7 +12267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>541</v>
       </c>
@@ -12358,7 +12355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>542</v>
       </c>
@@ -12446,7 +12443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>543</v>
       </c>
@@ -12534,7 +12531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>544</v>
       </c>
@@ -12622,7 +12619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>545</v>
       </c>
@@ -12710,7 +12707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>546</v>
       </c>
@@ -12798,7 +12795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>547</v>
       </c>
@@ -12886,7 +12883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>548</v>
       </c>
@@ -12974,7 +12971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>549</v>
       </c>
@@ -13062,7 +13059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>550</v>
       </c>
@@ -13150,7 +13147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>551</v>
       </c>
@@ -13238,7 +13235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>552</v>
       </c>
@@ -13326,7 +13323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>553</v>
       </c>
@@ -13414,7 +13411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>554</v>
       </c>
@@ -13502,7 +13499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>555</v>
       </c>
@@ -13590,7 +13587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>556</v>
       </c>
@@ -13678,7 +13675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>557</v>
       </c>
@@ -13766,7 +13763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>558</v>
       </c>
@@ -13854,7 +13851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>559</v>
       </c>
@@ -13942,7 +13939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>560</v>
       </c>
@@ -14030,7 +14027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>561</v>
       </c>
@@ -14118,7 +14115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>562</v>
       </c>
@@ -14206,7 +14203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>563</v>
       </c>
@@ -14294,7 +14291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>564</v>
       </c>
@@ -14382,7 +14379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>565</v>
       </c>
@@ -14470,7 +14467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>566</v>
       </c>
@@ -14558,7 +14555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>567</v>
       </c>
@@ -14646,7 +14643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>568</v>
       </c>
@@ -14734,7 +14731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>569</v>
       </c>
@@ -14822,7 +14819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>570</v>
       </c>
@@ -14910,7 +14907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>571</v>
       </c>
@@ -14998,7 +14995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>572</v>
       </c>
@@ -15086,7 +15083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>573</v>
       </c>
@@ -15174,7 +15171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>574</v>
       </c>
@@ -15262,7 +15259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>575</v>
       </c>
@@ -15350,7 +15347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>576</v>
       </c>
@@ -15438,7 +15435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>577</v>
       </c>
@@ -15526,7 +15523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>578</v>
       </c>
@@ -15614,7 +15611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>579</v>
       </c>
@@ -15702,7 +15699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>580</v>
       </c>
@@ -15790,7 +15787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>581</v>
       </c>
@@ -15878,7 +15875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>582</v>
       </c>
@@ -15966,7 +15963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>583</v>
       </c>
@@ -16054,7 +16051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>584</v>
       </c>
@@ -16142,7 +16139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>585</v>
       </c>
@@ -16230,7 +16227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>586</v>
       </c>
@@ -16318,7 +16315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>587</v>
       </c>
@@ -16406,7 +16403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>588</v>
       </c>
@@ -16494,7 +16491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>589</v>
       </c>
@@ -16582,7 +16579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>590</v>
       </c>
@@ -16670,7 +16667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>591</v>
       </c>
@@ -16758,7 +16755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>592</v>
       </c>
@@ -16846,7 +16843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>593</v>
       </c>
@@ -16934,7 +16931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>594</v>
       </c>
@@ -17022,7 +17019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>595</v>
       </c>
@@ -17110,7 +17107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>596</v>
       </c>
@@ -17198,7 +17195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>597</v>
       </c>
@@ -17286,7 +17283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>598</v>
       </c>
@@ -17374,7 +17371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>599</v>
       </c>
@@ -17462,7 +17459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>600</v>
       </c>
@@ -17550,7 +17547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>601</v>
       </c>
@@ -17638,7 +17635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>602</v>
       </c>
@@ -17726,7 +17723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>603</v>
       </c>
@@ -17814,7 +17811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>604</v>
       </c>
@@ -17902,7 +17899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>605</v>
       </c>
@@ -17990,7 +17987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>606</v>
       </c>
@@ -18078,7 +18075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>607</v>
       </c>
@@ -18166,7 +18163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>608</v>
       </c>
@@ -18254,7 +18251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>609</v>
       </c>
@@ -18342,7 +18339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>610</v>
       </c>
@@ -18430,7 +18427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>611</v>
       </c>
@@ -18518,7 +18515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>612</v>
       </c>
@@ -18606,7 +18603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>613</v>
       </c>
@@ -18694,7 +18691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>614</v>
       </c>
@@ -18782,7 +18779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>615</v>
       </c>
@@ -18870,7 +18867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>616</v>
       </c>
@@ -18958,7 +18955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>617</v>
       </c>
@@ -19046,7 +19043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>618</v>
       </c>
@@ -19134,7 +19131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>619</v>
       </c>
@@ -19222,7 +19219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>620</v>
       </c>
@@ -19310,7 +19307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>621</v>
       </c>
@@ -19398,7 +19395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>622</v>
       </c>
@@ -19486,7 +19483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>623</v>
       </c>
@@ -19574,7 +19571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>624</v>
       </c>
@@ -19662,7 +19659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>625</v>
       </c>
@@ -19750,7 +19747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>626</v>
       </c>
@@ -19838,7 +19835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>627</v>
       </c>
@@ -19926,7 +19923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>628</v>
       </c>
@@ -20014,7 +20011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>629</v>
       </c>
@@ -20102,7 +20099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>630</v>
       </c>
@@ -20190,7 +20187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>631</v>
       </c>
@@ -20278,7 +20275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>632</v>
       </c>
@@ -20366,7 +20363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>633</v>
       </c>
@@ -20454,7 +20451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>634</v>
       </c>
@@ -20542,7 +20539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>635</v>
       </c>
@@ -20630,7 +20627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>636</v>
       </c>
@@ -20718,7 +20715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>637</v>
       </c>
@@ -20806,7 +20803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>638</v>
       </c>
@@ -20894,7 +20891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>639</v>
       </c>
@@ -20982,7 +20979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>640</v>
       </c>
@@ -21070,7 +21067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>641</v>
       </c>
@@ -21158,7 +21155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>642</v>
       </c>
@@ -21246,7 +21243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>643</v>
       </c>
@@ -21334,7 +21331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>644</v>
       </c>
@@ -21422,7 +21419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>645</v>
       </c>
@@ -21510,7 +21507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>646</v>
       </c>
@@ -21598,7 +21595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>647</v>
       </c>
@@ -21686,7 +21683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>648</v>
       </c>
@@ -21774,7 +21771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>649</v>
       </c>
@@ -21862,7 +21859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>650</v>
       </c>
@@ -21950,7 +21947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>651</v>
       </c>
@@ -22038,7 +22035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>652</v>
       </c>
@@ -22126,7 +22123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>653</v>
       </c>
@@ -22214,7 +22211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>654</v>
       </c>
@@ -22302,7 +22299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>655</v>
       </c>
@@ -22390,7 +22387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>656</v>
       </c>
@@ -22478,7 +22475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>657</v>
       </c>
@@ -22566,7 +22563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>658</v>
       </c>
@@ -22654,7 +22651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>659</v>
       </c>
@@ -22742,7 +22739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>660</v>
       </c>
@@ -22830,7 +22827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A212" s="25" t="s">
         <v>661</v>
       </c>
@@ -22918,7 +22915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A213" s="25" t="s">
         <v>662</v>
       </c>
@@ -23006,7 +23003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A214" s="25" t="s">
         <v>663</v>
       </c>
@@ -23094,7 +23091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A215" s="25" t="s">
         <v>664</v>
       </c>
@@ -23182,7 +23179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A216" s="13" t="s">
         <v>665</v>
       </c>
@@ -23270,7 +23267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A217" s="13" t="s">
         <v>666</v>
       </c>
@@ -23358,7 +23355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>667</v>
       </c>
@@ -23446,7 +23443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A219" s="23" t="s">
         <v>668</v>
       </c>
@@ -23534,7 +23531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A220" s="23" t="s">
         <v>669</v>
       </c>
@@ -23622,7 +23619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A221" s="23" t="s">
         <v>670</v>
       </c>
@@ -23710,7 +23707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A222" s="23" t="s">
         <v>671</v>
       </c>
@@ -23798,7 +23795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A223" s="23" t="s">
         <v>672</v>
       </c>
@@ -23886,7 +23883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A224" s="22" t="s">
         <v>673</v>
       </c>
@@ -23974,7 +23971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A225" s="22" t="s">
         <v>674</v>
       </c>
@@ -24062,7 +24059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A226" s="22" t="s">
         <v>675</v>
       </c>
@@ -24150,7 +24147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A227" s="22" t="s">
         <v>676</v>
       </c>
@@ -24238,7 +24235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A228" s="24" t="s">
         <v>677</v>
       </c>
@@ -24326,7 +24323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A229" s="24" t="s">
         <v>678</v>
       </c>
@@ -24414,7 +24411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A230" s="24" t="s">
         <v>679</v>
       </c>
@@ -24502,7 +24499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A231" s="24" t="s">
         <v>680</v>
       </c>
@@ -24590,7 +24587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A232" s="24" t="s">
         <v>681</v>
       </c>
@@ -24678,7 +24675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A233" s="24" t="s">
         <v>682</v>
       </c>
@@ -24766,7 +24763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A234" s="24" t="s">
         <v>683</v>
       </c>
@@ -24854,7 +24851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A235" s="24" t="s">
         <v>684</v>
       </c>
@@ -24942,7 +24939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>685</v>
       </c>
@@ -25030,7 +25027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>686</v>
       </c>
@@ -25118,7 +25115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>687</v>
       </c>
@@ -25206,7 +25203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>688</v>
       </c>
@@ -25294,7 +25291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>689</v>
       </c>
@@ -25382,7 +25379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>690</v>
       </c>
@@ -25470,7 +25467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>691</v>
       </c>
@@ -25558,7 +25555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>692</v>
       </c>
@@ -25646,7 +25643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>693</v>
       </c>
@@ -25734,7 +25731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>694</v>
       </c>
@@ -25822,7 +25819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>695</v>
       </c>
@@ -25910,7 +25907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>696</v>
       </c>
@@ -25998,7 +25995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>697</v>
       </c>
@@ -26086,7 +26083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>698</v>
       </c>
@@ -26174,7 +26171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A250" s="26" t="s">
         <v>699</v>
       </c>
@@ -26262,7 +26259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>700</v>
       </c>
@@ -26350,7 +26347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>701</v>
       </c>
@@ -26438,7 +26435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>702</v>
       </c>
@@ -26526,7 +26523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>703</v>
       </c>
@@ -26614,7 +26611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>704</v>
       </c>
@@ -26702,7 +26699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>705</v>
       </c>
@@ -26790,7 +26787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>706</v>
       </c>
@@ -26878,7 +26875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A258" s="16" t="s">
         <v>707</v>
       </c>
@@ -26966,7 +26963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>708</v>
       </c>
@@ -27054,7 +27051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>709</v>
       </c>
@@ -27142,7 +27139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A261" s="16" t="s">
         <v>710</v>
       </c>
@@ -27230,7 +27227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A262" s="16" t="s">
         <v>711</v>
       </c>
@@ -27318,7 +27315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A263" s="15" t="s">
         <v>712</v>
       </c>
@@ -27406,7 +27403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A264" s="15" t="s">
         <v>713</v>
       </c>
@@ -27494,7 +27491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A265" s="15" t="s">
         <v>714</v>
       </c>
@@ -27582,7 +27579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A266" s="15" t="s">
         <v>715</v>
       </c>
@@ -27670,7 +27667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A267" s="15" t="s">
         <v>716</v>
       </c>
@@ -27758,7 +27755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>717</v>
       </c>
@@ -27846,7 +27843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>718</v>
       </c>
@@ -27934,7 +27931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>719</v>
       </c>
@@ -28022,7 +28019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>720</v>
       </c>
@@ -28110,7 +28107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>721</v>
       </c>
@@ -28198,7 +28195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>722</v>
       </c>
@@ -28286,7 +28283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>723</v>
       </c>
@@ -28374,7 +28371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>724</v>
       </c>
@@ -28462,7 +28459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>725</v>
       </c>
@@ -28550,7 +28547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>726</v>
       </c>
@@ -28638,7 +28635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A278" s="27" t="s">
         <v>727</v>
       </c>
@@ -28726,7 +28723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>728</v>
       </c>
@@ -28814,7 +28811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A280" s="18" t="s">
         <v>729</v>
       </c>
@@ -28902,7 +28899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A281" s="18" t="s">
         <v>730</v>
       </c>
@@ -28990,7 +28987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A282" s="18" t="s">
         <v>731</v>
       </c>
@@ -29078,7 +29075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A283" s="18" t="s">
         <v>732</v>
       </c>
@@ -29166,7 +29163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A284" s="18" t="s">
         <v>733</v>
       </c>
@@ -29254,7 +29251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>734</v>
       </c>
@@ -29342,7 +29339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A286" s="19" t="s">
         <v>735</v>
       </c>
@@ -29430,7 +29427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A287" s="19" t="s">
         <v>736</v>
       </c>
@@ -29518,7 +29515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A288" s="19" t="s">
         <v>737</v>
       </c>
@@ -29606,7 +29603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A289" s="19" t="s">
         <v>738</v>
       </c>
@@ -29694,7 +29691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A290" s="19" t="s">
         <v>739</v>
       </c>
@@ -29782,7 +29779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>740</v>
       </c>
@@ -29870,7 +29867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>741</v>
       </c>
@@ -29958,7 +29955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>742</v>
       </c>
@@ -30046,7 +30043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>743</v>
       </c>
@@ -30134,7 +30131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>744</v>
       </c>
@@ -30222,7 +30219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>745</v>
       </c>
@@ -30310,7 +30307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A297" s="17" t="s">
         <v>746</v>
       </c>
@@ -30398,7 +30395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A298" s="17" t="s">
         <v>747</v>
       </c>
@@ -30486,7 +30483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A299" s="17" t="s">
         <v>748</v>
       </c>
@@ -30574,7 +30571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A300" s="17" t="s">
         <v>749</v>
       </c>
@@ -30662,7 +30659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A301" s="17" t="s">
         <v>750</v>
       </c>
@@ -30750,7 +30747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A302" s="17" t="s">
         <v>751</v>
       </c>
@@ -30838,7 +30835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A303" s="17" t="s">
         <v>752</v>
       </c>
@@ -30926,7 +30923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A304" s="17" t="s">
         <v>753</v>
       </c>
@@ -31014,7 +31011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A305" s="17" t="s">
         <v>754</v>
       </c>
@@ -31102,7 +31099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A306" s="17" t="s">
         <v>755</v>
       </c>
@@ -31190,7 +31187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A307" s="26" t="s">
         <v>756</v>
       </c>
@@ -31278,7 +31275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A308" s="26" t="s">
         <v>757</v>
       </c>
@@ -31366,7 +31363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A309" s="26" t="s">
         <v>758</v>
       </c>
@@ -31454,7 +31451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A310" s="26" t="s">
         <v>759</v>
       </c>
@@ -31542,7 +31539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A311" s="26" t="s">
         <v>760</v>
       </c>
@@ -31630,7 +31627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A312" s="26" t="s">
         <v>761</v>
       </c>
@@ -31718,7 +31715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A313" s="15" t="s">
         <v>762</v>
       </c>
@@ -31806,7 +31803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>763</v>
       </c>
@@ -31894,7 +31891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>764</v>
       </c>
@@ -31982,7 +31979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>765</v>
       </c>
@@ -32070,7 +32067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>766</v>
       </c>
@@ -32158,7 +32155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>767</v>
       </c>
@@ -32246,7 +32243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>768</v>
       </c>
@@ -32334,7 +32331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>769</v>
       </c>
@@ -32422,7 +32419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>770</v>
       </c>
@@ -32510,7 +32507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>771</v>
       </c>
@@ -32598,7 +32595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>772</v>
       </c>
@@ -32686,7 +32683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>773</v>
       </c>
@@ -32774,7 +32771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>774</v>
       </c>
@@ -32862,7 +32859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>775</v>
       </c>
@@ -32950,7 +32947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>776</v>
       </c>
@@ -33038,7 +33035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>777</v>
       </c>
@@ -33126,7 +33123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>778</v>
       </c>
@@ -33214,7 +33211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>779</v>
       </c>
@@ -33302,7 +33299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>780</v>
       </c>
@@ -33390,7 +33387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>781</v>
       </c>
@@ -33478,7 +33475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>782</v>
       </c>
@@ -33566,7 +33563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>783</v>
       </c>
@@ -33654,7 +33651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>784</v>
       </c>
@@ -33742,7 +33739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>785</v>
       </c>
@@ -33830,7 +33827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>786</v>
       </c>
@@ -33918,7 +33915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>787</v>
       </c>
@@ -34006,7 +34003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>788</v>
       </c>
@@ -34094,7 +34091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>789</v>
       </c>
@@ -34182,7 +34179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>790</v>
       </c>
@@ -34270,7 +34267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>791</v>
       </c>
@@ -34358,7 +34355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>792</v>
       </c>
@@ -34446,7 +34443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>793</v>
       </c>
@@ -34534,7 +34531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>794</v>
       </c>
@@ -34622,7 +34619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>795</v>
       </c>
@@ -34710,7 +34707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>796</v>
       </c>
@@ -34798,7 +34795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>797</v>
       </c>
@@ -34886,7 +34883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>798</v>
       </c>
@@ -34974,7 +34971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>799</v>
       </c>
@@ -35062,7 +35059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>800</v>
       </c>
@@ -35150,7 +35147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>801</v>
       </c>
@@ -35238,7 +35235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>802</v>
       </c>
@@ -35326,7 +35323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>803</v>
       </c>
@@ -35414,7 +35411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>804</v>
       </c>
@@ -35502,7 +35499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>805</v>
       </c>
@@ -35590,7 +35587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>806</v>
       </c>
@@ -35678,7 +35675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>807</v>
       </c>
@@ -35766,7 +35763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>808</v>
       </c>
@@ -35854,7 +35851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>809</v>
       </c>
@@ -35942,7 +35939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>810</v>
       </c>
@@ -36030,7 +36027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>811</v>
       </c>
@@ -36118,7 +36115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>812</v>
       </c>
@@ -36206,7 +36203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>813</v>
       </c>
@@ -36294,7 +36291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>814</v>
       </c>
@@ -36382,7 +36379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>815</v>
       </c>
@@ -36470,7 +36467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>816</v>
       </c>
@@ -36558,7 +36555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>817</v>
       </c>
@@ -36646,7 +36643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>818</v>
       </c>
@@ -36734,7 +36731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>819</v>
       </c>
@@ -36822,7 +36819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>820</v>
       </c>
@@ -36910,7 +36907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>821</v>
       </c>
@@ -36998,7 +36995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>822</v>
       </c>
@@ -37086,7 +37083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>823</v>
       </c>
@@ -37174,7 +37171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>824</v>
       </c>
@@ -37262,7 +37259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>825</v>
       </c>
@@ -37350,7 +37347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>826</v>
       </c>
@@ -37438,7 +37435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>827</v>
       </c>
@@ -37526,7 +37523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>828</v>
       </c>
@@ -37614,7 +37611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>829</v>
       </c>
@@ -37702,7 +37699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>830</v>
       </c>
@@ -37790,7 +37787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>831</v>
       </c>
@@ -37878,7 +37875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>832</v>
       </c>
@@ -37966,7 +37963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>833</v>
       </c>
@@ -38054,7 +38051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>834</v>
       </c>
@@ -38142,7 +38139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>835</v>
       </c>
@@ -38230,7 +38227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>836</v>
       </c>
@@ -38318,7 +38315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>837</v>
       </c>
@@ -38406,7 +38403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>838</v>
       </c>
@@ -38494,7 +38491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>839</v>
       </c>
@@ -38582,7 +38579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>840</v>
       </c>
@@ -38670,7 +38667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>841</v>
       </c>
@@ -38758,7 +38755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>842</v>
       </c>
@@ -38846,7 +38843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>843</v>
       </c>
@@ -38934,7 +38931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>844</v>
       </c>
@@ -39022,7 +39019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>845</v>
       </c>
@@ -39110,7 +39107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>846</v>
       </c>
@@ -39198,7 +39195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>847</v>
       </c>
@@ -39286,7 +39283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>848</v>
       </c>
@@ -39374,7 +39371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>849</v>
       </c>
@@ -39462,7 +39459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>850</v>
       </c>
@@ -39550,7 +39547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>851</v>
       </c>
@@ -39638,7 +39635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>852</v>
       </c>
@@ -39726,7 +39723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>853</v>
       </c>
@@ -39814,7 +39811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>854</v>
       </c>
@@ -39902,7 +39899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>855</v>
       </c>
@@ -39990,7 +39987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>856</v>
       </c>
@@ -40078,7 +40075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>857</v>
       </c>
@@ -40166,7 +40163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>858</v>
       </c>
@@ -40254,7 +40251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>859</v>
       </c>
@@ -40342,7 +40339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>860</v>
       </c>
@@ -40430,7 +40427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>861</v>
       </c>
@@ -40518,7 +40515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>862</v>
       </c>
@@ -40606,7 +40603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>863</v>
       </c>
@@ -40694,7 +40691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>864</v>
       </c>
@@ -40782,7 +40779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>865</v>
       </c>
@@ -40870,7 +40867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>866</v>
       </c>
@@ -40958,7 +40955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>867</v>
       </c>
@@ -41046,7 +41043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>868</v>
       </c>
@@ -41134,7 +41131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>869</v>
       </c>
@@ -41220,7 +41217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>870</v>
       </c>
@@ -41306,7 +41303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>871</v>
       </c>
@@ -41392,7 +41389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>872</v>
       </c>
@@ -41478,7 +41475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>873</v>
       </c>
@@ -41566,7 +41563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>874</v>
       </c>
@@ -41654,7 +41651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>875</v>
       </c>
@@ -41742,7 +41739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>876</v>
       </c>
@@ -41830,7 +41827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>877</v>
       </c>
@@ -41918,7 +41915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>878</v>
       </c>
@@ -42006,7 +42003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>879</v>
       </c>
@@ -42094,7 +42091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>880</v>
       </c>
@@ -42182,7 +42179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
         <v>881</v>
       </c>
@@ -42634,29 +42631,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB70D1E-F6AB-4CF2-AC07-C4E56376D886}">
   <dimension ref="A2:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="4" max="20" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="20" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="40" t="s">
         <v>903</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="41" t="s">
         <v>904</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D6" s="42" t="s">
         <v>905</v>
       </c>
@@ -42700,7 +42697,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D7" s="42" t="s">
         <v>919</v>
       </c>
@@ -42744,7 +42741,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" s="43" t="s">
         <v>907</v>
       </c>
@@ -42794,7 +42791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" s="43" t="s">
         <v>933</v>
       </c>
@@ -42844,7 +42841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" s="43" t="s">
         <v>935</v>
       </c>
@@ -42894,7 +42891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="43" t="s">
         <v>937</v>
       </c>
@@ -42944,7 +42941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" s="43" t="s">
         <v>939</v>
       </c>
@@ -42994,7 +42991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -43047,7 +43044,7 @@
         <v>0.94166040230902204</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -43100,7 +43097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -43153,7 +43150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -43206,7 +43203,7 @@
         <v>0.95200977870694903</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -43259,7 +43256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -43312,7 +43309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -43365,7 +43362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -43418,7 +43415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -43439,7 +43436,7 @@
       <c r="P21" s="51"/>
       <c r="Q21" s="53"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -43492,7 +43489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -43545,7 +43542,7 @@
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
@@ -43598,7 +43595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
@@ -43651,7 +43648,7 @@
         <v>0.94234466577596099</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -43704,7 +43701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>27</v>
       </c>
@@ -43757,7 +43754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>28</v>
       </c>
@@ -43810,7 +43807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>29</v>
       </c>
@@ -43863,25 +43860,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="P30" s="65"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="41" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D34" s="77" t="s">
         <v>956</v>
       </c>
@@ -43910,7 +43907,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>958</v>
       </c>
@@ -43921,7 +43918,7 @@
         <v>311</v>
       </c>
       <c r="F35" t="s">
-        <v>959</v>
+        <v>885</v>
       </c>
       <c r="G35" t="s">
         <v>883</v>
@@ -43969,9 +43966,9 @@
         <v>289</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="44" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B36" s="43" t="s">
         <v>546</v>
@@ -44007,9 +44004,9 @@
       <c r="T36" s="67"/>
       <c r="U36" s="68"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="44" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B37" s="43" t="s">
         <v>547</v>
@@ -44045,9 +44042,9 @@
       <c r="T37" s="70"/>
       <c r="U37" s="71"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="44" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B38" s="43" t="s">
         <v>548</v>
@@ -44083,9 +44080,9 @@
       <c r="T38" s="70"/>
       <c r="U38" s="71"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="44" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B39" s="43" t="s">
         <v>549</v>
@@ -44121,9 +44118,9 @@
       <c r="T39" s="70"/>
       <c r="U39" s="71"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="44" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B40" s="43" t="s">
         <v>554</v>
@@ -44159,9 +44156,9 @@
       <c r="T40" s="70"/>
       <c r="U40" s="71"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B41" s="43" t="s">
         <v>607</v>
@@ -44209,9 +44206,9 @@
       <c r="T41" s="70"/>
       <c r="U41" s="71"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B42" s="43" t="s">
         <v>608</v>
@@ -44259,9 +44256,9 @@
       <c r="T42" s="70"/>
       <c r="U42" s="71"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B43" s="43" t="s">
         <v>609</v>
@@ -44309,9 +44306,9 @@
       <c r="T43" s="70"/>
       <c r="U43" s="71"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B44" s="43" t="s">
         <v>610</v>
@@ -44359,9 +44356,9 @@
       <c r="T44" s="70"/>
       <c r="U44" s="71"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B45" s="43" t="s">
         <v>621</v>
@@ -44424,9 +44421,9 @@
       <c r="T45" s="70"/>
       <c r="U45" s="71"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B46" s="43" t="s">
         <v>622</v>
@@ -44489,9 +44486,9 @@
       <c r="T46" s="70"/>
       <c r="U46" s="71"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B47" s="43" t="s">
         <v>623</v>
@@ -44554,9 +44551,9 @@
       <c r="T47" s="70"/>
       <c r="U47" s="71"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B48" s="43" t="s">
         <v>624</v>
@@ -44619,9 +44616,9 @@
       <c r="T48" s="70"/>
       <c r="U48" s="71"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B49" s="43" t="s">
         <v>625</v>
@@ -44684,9 +44681,9 @@
       <c r="T49" s="70"/>
       <c r="U49" s="71"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B50" s="43" t="s">
         <v>627</v>
@@ -44749,9 +44746,9 @@
       <c r="T50" s="70"/>
       <c r="U50" s="71"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B51" s="43" t="s">
         <v>626</v>
@@ -44814,9 +44811,9 @@
       <c r="T51" s="70"/>
       <c r="U51" s="71"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B52" s="43" t="s">
         <v>628</v>
@@ -44879,9 +44876,9 @@
       <c r="T52" s="70"/>
       <c r="U52" s="71"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B53" s="43" t="s">
         <v>629</v>
@@ -44944,9 +44941,9 @@
       <c r="T53" s="70"/>
       <c r="U53" s="71"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B54" s="43" t="s">
         <v>630</v>
@@ -45009,9 +45006,9 @@
       <c r="T54" s="70"/>
       <c r="U54" s="71"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B55" s="43" t="s">
         <v>631</v>
@@ -45074,9 +45071,9 @@
       <c r="T55" s="70"/>
       <c r="U55" s="71"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B56" s="43" t="s">
         <v>632</v>
@@ -45139,9 +45136,9 @@
       <c r="T56" s="70"/>
       <c r="U56" s="71"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B57" s="43" t="s">
         <v>633</v>
@@ -45204,9 +45201,9 @@
       <c r="T57" s="70"/>
       <c r="U57" s="71"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B58" s="43" t="s">
         <v>634</v>
@@ -45269,9 +45266,9 @@
       <c r="T58" s="70"/>
       <c r="U58" s="71"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="49" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B59" s="43" t="s">
         <v>578</v>
@@ -45322,9 +45319,9 @@
       <c r="T59" s="70"/>
       <c r="U59" s="71"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="49" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B60" s="43" t="s">
         <v>579</v>
@@ -45405,9 +45402,9 @@
       <selection sqref="A1:T26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="75" t="str">
         <f>exio_usa!B35</f>
         <v>USA</v>
@@ -45426,7 +45423,7 @@
       </c>
       <c r="E1" s="75" t="str">
         <f>exio_usa!F35</f>
-        <v>Other buildungs</v>
+        <v>Other buildings</v>
       </c>
       <c r="F1" s="75" t="str">
         <f>exio_usa!G35</f>
@@ -45489,7 +45486,7 @@
         <v>Services</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="75" t="str">
         <f>exio_usa!B36</f>
         <v>321100</v>
@@ -45571,7 +45568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="75" t="str">
         <f>exio_usa!B37</f>
         <v>321219</v>
@@ -45653,7 +45650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="75" t="str">
         <f>exio_usa!B38</f>
         <v>32121A</v>
@@ -45735,7 +45732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="75" t="str">
         <f>exio_usa!B39</f>
         <v>32121B</v>
@@ -45817,7 +45814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="75" t="str">
         <f>exio_usa!B40</f>
         <v>321999</v>
@@ -45899,7 +45896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="75" t="str">
         <f>exio_usa!B41</f>
         <v>327211</v>
@@ -45981,7 +45978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="75" t="str">
         <f>exio_usa!B42</f>
         <v>327212</v>
@@ -46063,7 +46060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="75" t="str">
         <f>exio_usa!B43</f>
         <v>327213</v>
@@ -46145,7 +46142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="75" t="str">
         <f>exio_usa!B44</f>
         <v>327215</v>
@@ -46227,7 +46224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="75" t="str">
         <f>exio_usa!B45</f>
         <v>331110</v>
@@ -46309,7 +46306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="75" t="str">
         <f>exio_usa!B46</f>
         <v>331200</v>
@@ -46391,7 +46388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="75" t="str">
         <f>exio_usa!B47</f>
         <v>331314</v>
@@ -46473,7 +46470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="75" t="str">
         <f>exio_usa!B48</f>
         <v>33131A</v>
@@ -46555,7 +46552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="75" t="str">
         <f>exio_usa!B49</f>
         <v>33131B</v>
@@ -46637,7 +46634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="75" t="str">
         <f>exio_usa!B50</f>
         <v>331419</v>
@@ -46719,7 +46716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="75" t="str">
         <f>exio_usa!B51</f>
         <v>331411</v>
@@ -46801,7 +46798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="75" t="str">
         <f>exio_usa!B52</f>
         <v>331420</v>
@@ -46883,7 +46880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="75" t="str">
         <f>exio_usa!B53</f>
         <v>331490</v>
@@ -46965,7 +46962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="75" t="str">
         <f>exio_usa!B54</f>
         <v>331510</v>
@@ -47047,7 +47044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="75" t="str">
         <f>exio_usa!B55</f>
         <v>331520</v>
@@ -47129,7 +47126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="75" t="str">
         <f>exio_usa!B56</f>
         <v>332114</v>
@@ -47211,7 +47208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="75" t="str">
         <f>exio_usa!B57</f>
         <v>33211A</v>
@@ -47293,7 +47290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="75" t="str">
         <f>exio_usa!B58</f>
         <v>33211B</v>
@@ -47375,7 +47372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="75" t="str">
         <f>exio_usa!B59</f>
         <v>325211</v>
@@ -47457,7 +47454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="75" t="str">
         <f>exio_usa!B60</f>
         <v>325212</v>

</xml_diff>